<commit_message>
Commit 20171025 -fin del dia-
Avance a estandarización del dataset PIGOO
</commit_message>
<xml_diff>
--- a/Datasets/Pigoo/CiudadesPIGOO_ClaveInegi.xlsx
+++ b/Datasets/Pigoo/CiudadesPIGOO_ClaveInegi.xlsx
@@ -15,7 +15,7 @@
     <sheet name="OOAPAS-PIGOO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'OOAPAS-PIGOO'!$B$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'OOAPAS-PIGOO'!$B$1:$J$246</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -2878,13 +2878,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:L246"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E153" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F187" sqref="F187"/>
+      <selection pane="bottomRight" activeCell="C255" sqref="C255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2933,7 +2934,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2962,7 +2963,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2991,7 +2992,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3020,7 +3021,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3049,7 +3050,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3078,7 +3079,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3107,7 +3108,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3136,7 +3137,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3165,7 +3166,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3194,7 +3195,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3223,7 +3224,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3252,7 +3253,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3281,7 +3282,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3310,7 +3311,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3339,7 +3340,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3368,7 +3369,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3397,7 +3398,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3426,7 +3427,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3455,7 +3456,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3484,7 +3485,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3513,7 +3514,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3542,7 +3543,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3571,7 +3572,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3600,7 +3601,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3629,7 +3630,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3658,7 +3659,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3687,7 +3688,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3716,7 +3717,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3745,7 +3746,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3774,7 +3775,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3803,7 +3804,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3832,7 +3833,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3861,7 +3862,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3890,7 +3891,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3919,7 +3920,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3948,7 +3949,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3978,7 +3979,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4008,7 +4009,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4037,7 +4038,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4066,7 +4067,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4095,7 +4096,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4124,7 +4125,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4151,7 +4152,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4180,7 +4181,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4209,7 +4210,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4239,7 +4240,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4268,7 +4269,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4297,7 +4298,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4326,7 +4327,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4355,7 +4356,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4384,7 +4385,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4413,7 +4414,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4442,7 +4443,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4471,7 +4472,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4500,7 +4501,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4530,7 +4531,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4559,7 +4560,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4588,7 +4589,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4617,7 +4618,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4646,7 +4647,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4675,7 +4676,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4704,7 +4705,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4733,7 +4734,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4762,7 +4763,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4791,7 +4792,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4820,7 +4821,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4849,7 +4850,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4878,7 +4879,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4907,7 +4908,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4936,7 +4937,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4965,7 +4966,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4994,7 +4995,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -5023,7 +5024,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -5052,7 +5053,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -5081,7 +5082,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -5110,7 +5111,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -5139,7 +5140,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -5168,7 +5169,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -5197,7 +5198,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -5226,7 +5227,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -5255,7 +5256,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -5284,7 +5285,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -5313,7 +5314,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -5342,7 +5343,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -5371,7 +5372,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -5400,7 +5401,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -5429,7 +5430,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -5458,7 +5459,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -5487,7 +5488,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -5516,7 +5517,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -5545,7 +5546,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -5574,7 +5575,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -5603,7 +5604,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
@@ -5632,7 +5633,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -5661,7 +5662,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
@@ -5690,7 +5691,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>96</v>
       </c>
@@ -5719,7 +5720,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>97</v>
       </c>
@@ -5748,7 +5749,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>98</v>
       </c>
@@ -5777,7 +5778,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>99</v>
       </c>
@@ -5807,7 +5808,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>100</v>
       </c>
@@ -5836,7 +5837,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>101</v>
       </c>
@@ -5865,7 +5866,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>102</v>
       </c>
@@ -5894,7 +5895,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>103</v>
       </c>
@@ -5923,7 +5924,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>104</v>
       </c>
@@ -5953,7 +5954,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>105</v>
       </c>
@@ -5982,7 +5983,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>106</v>
       </c>
@@ -6011,7 +6012,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>107</v>
       </c>
@@ -6040,7 +6041,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>108</v>
       </c>
@@ -6069,7 +6070,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>109</v>
       </c>
@@ -6098,7 +6099,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>110</v>
       </c>
@@ -6127,7 +6128,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>111</v>
       </c>
@@ -6156,7 +6157,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>112</v>
       </c>
@@ -6185,7 +6186,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>113</v>
       </c>
@@ -6214,7 +6215,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>114</v>
       </c>
@@ -6243,7 +6244,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>115</v>
       </c>
@@ -6272,7 +6273,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>116</v>
       </c>
@@ -6301,7 +6302,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>117</v>
       </c>
@@ -6330,7 +6331,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>118</v>
       </c>
@@ -6359,7 +6360,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>119</v>
       </c>
@@ -6388,7 +6389,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>120</v>
       </c>
@@ -6417,7 +6418,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>121</v>
       </c>
@@ -6446,7 +6447,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>122</v>
       </c>
@@ -6475,7 +6476,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>123</v>
       </c>
@@ -6504,7 +6505,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>124</v>
       </c>
@@ -6533,7 +6534,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>125</v>
       </c>
@@ -6562,7 +6563,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>126</v>
       </c>
@@ -6591,7 +6592,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>127</v>
       </c>
@@ -6620,7 +6621,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>128</v>
       </c>
@@ -6649,7 +6650,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>129</v>
       </c>
@@ -6678,7 +6679,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>130</v>
       </c>
@@ -6707,7 +6708,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>131</v>
       </c>
@@ -6736,7 +6737,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>132</v>
       </c>
@@ -6765,7 +6766,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>133</v>
       </c>
@@ -6794,7 +6795,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>134</v>
       </c>
@@ -6823,7 +6824,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>135</v>
       </c>
@@ -6852,7 +6853,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>136</v>
       </c>
@@ -6881,7 +6882,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>137</v>
       </c>
@@ -6910,7 +6911,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>138</v>
       </c>
@@ -6939,7 +6940,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>139</v>
       </c>
@@ -6968,7 +6969,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>140</v>
       </c>
@@ -6997,7 +6998,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>141</v>
       </c>
@@ -7026,7 +7027,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>142</v>
       </c>
@@ -7055,7 +7056,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>143</v>
       </c>
@@ -7084,7 +7085,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>144</v>
       </c>
@@ -7113,7 +7114,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>145</v>
       </c>
@@ -7142,7 +7143,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>146</v>
       </c>
@@ -7171,7 +7172,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>147</v>
       </c>
@@ -7200,7 +7201,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>148</v>
       </c>
@@ -7229,7 +7230,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>149</v>
       </c>
@@ -7261,7 +7262,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>150</v>
       </c>
@@ -7290,7 +7291,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>151</v>
       </c>
@@ -7319,7 +7320,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>152</v>
       </c>
@@ -7348,7 +7349,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>153</v>
       </c>
@@ -7377,7 +7378,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>154</v>
       </c>
@@ -7406,7 +7407,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>155</v>
       </c>
@@ -7435,7 +7436,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>156</v>
       </c>
@@ -7464,7 +7465,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="158" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:12" s="11" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>157</v>
       </c>
@@ -7496,7 +7497,7 @@
       <c r="K158"/>
       <c r="L158"/>
     </row>
-    <row r="159" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:12" s="11" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>158</v>
       </c>
@@ -7528,7 +7529,7 @@
       <c r="K159"/>
       <c r="L159"/>
     </row>
-    <row r="160" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:12" s="11" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>159</v>
       </c>
@@ -7560,7 +7561,7 @@
       <c r="K160"/>
       <c r="L160"/>
     </row>
-    <row r="161" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:12" s="11" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>160</v>
       </c>
@@ -7592,7 +7593,7 @@
       <c r="K161"/>
       <c r="L161"/>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>161</v>
       </c>
@@ -7621,7 +7622,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>162</v>
       </c>
@@ -7650,7 +7651,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>163</v>
       </c>
@@ -7679,7 +7680,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>164</v>
       </c>
@@ -7708,7 +7709,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>165</v>
       </c>
@@ -7737,7 +7738,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>166</v>
       </c>
@@ -7766,7 +7767,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>167</v>
       </c>
@@ -7795,7 +7796,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>168</v>
       </c>
@@ -7824,7 +7825,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>169</v>
       </c>
@@ -7853,7 +7854,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>170</v>
       </c>
@@ -7882,7 +7883,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>171</v>
       </c>
@@ -7911,7 +7912,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>172</v>
       </c>
@@ -7940,7 +7941,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>173</v>
       </c>
@@ -7969,7 +7970,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>174</v>
       </c>
@@ -7998,7 +7999,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>175</v>
       </c>
@@ -8028,7 +8029,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>176</v>
       </c>
@@ -8057,7 +8058,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>177</v>
       </c>
@@ -8086,7 +8087,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>178</v>
       </c>
@@ -8115,7 +8116,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>179</v>
       </c>
@@ -8147,7 +8148,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>180</v>
       </c>
@@ -8176,7 +8177,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>181</v>
       </c>
@@ -8205,7 +8206,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>182</v>
       </c>
@@ -8234,7 +8235,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>183</v>
       </c>
@@ -8263,7 +8264,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>184</v>
       </c>
@@ -8292,7 +8293,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>185</v>
       </c>
@@ -8321,7 +8322,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>186</v>
       </c>
@@ -8350,7 +8351,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>187</v>
       </c>
@@ -8379,7 +8380,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>188</v>
       </c>
@@ -8408,7 +8409,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>189</v>
       </c>
@@ -8437,7 +8438,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>190</v>
       </c>
@@ -8466,7 +8467,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>191</v>
       </c>
@@ -8495,7 +8496,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>192</v>
       </c>
@@ -8524,7 +8525,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>193</v>
       </c>
@@ -8553,7 +8554,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>194</v>
       </c>
@@ -8585,7 +8586,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>195</v>
       </c>
@@ -8614,7 +8615,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>196</v>
       </c>
@@ -8643,7 +8644,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>197</v>
       </c>
@@ -8672,7 +8673,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>198</v>
       </c>
@@ -8701,7 +8702,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>199</v>
       </c>
@@ -8730,7 +8731,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>200</v>
       </c>
@@ -8759,7 +8760,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>201</v>
       </c>
@@ -8788,7 +8789,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>202</v>
       </c>
@@ -8817,7 +8818,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>203</v>
       </c>
@@ -8847,7 +8848,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>204</v>
       </c>
@@ -8876,7 +8877,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>205</v>
       </c>
@@ -8905,7 +8906,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>206</v>
       </c>
@@ -8934,7 +8935,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>207</v>
       </c>
@@ -8963,7 +8964,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>208</v>
       </c>
@@ -8992,7 +8993,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>209</v>
       </c>
@@ -9021,7 +9022,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>210</v>
       </c>
@@ -9050,7 +9051,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>211</v>
       </c>
@@ -9079,7 +9080,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>212</v>
       </c>
@@ -9108,7 +9109,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>213</v>
       </c>
@@ -9137,7 +9138,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>214</v>
       </c>
@@ -9166,7 +9167,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>215</v>
       </c>
@@ -9195,7 +9196,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>216</v>
       </c>
@@ -9224,7 +9225,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>217</v>
       </c>
@@ -9253,7 +9254,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>218</v>
       </c>
@@ -9282,7 +9283,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>219</v>
       </c>
@@ -9311,7 +9312,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>220</v>
       </c>
@@ -9340,7 +9341,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>221</v>
       </c>
@@ -9369,7 +9370,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>222</v>
       </c>
@@ -9398,7 +9399,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>223</v>
       </c>
@@ -9427,7 +9428,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>224</v>
       </c>
@@ -9456,7 +9457,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>225</v>
       </c>
@@ -9486,7 +9487,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>226</v>
       </c>
@@ -9515,7 +9516,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>227</v>
       </c>
@@ -9544,7 +9545,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>228</v>
       </c>
@@ -9573,7 +9574,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>229</v>
       </c>
@@ -9602,7 +9603,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>230</v>
       </c>
@@ -9631,7 +9632,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>231</v>
       </c>
@@ -9660,7 +9661,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>232</v>
       </c>
@@ -9689,7 +9690,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>233</v>
       </c>
@@ -9718,7 +9719,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>234</v>
       </c>
@@ -9747,7 +9748,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>235</v>
       </c>
@@ -9776,7 +9777,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>236</v>
       </c>
@@ -9805,7 +9806,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>237</v>
       </c>
@@ -9834,7 +9835,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>238</v>
       </c>
@@ -9863,7 +9864,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>239</v>
       </c>
@@ -9892,7 +9893,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>240</v>
       </c>
@@ -9921,7 +9922,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>241</v>
       </c>
@@ -9950,7 +9951,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>242</v>
       </c>
@@ -9979,7 +9980,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>243</v>
       </c>
@@ -10008,7 +10009,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>244</v>
       </c>
@@ -10068,10 +10069,12 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:J1">
-    <sortState ref="B2:J246">
-      <sortCondition ref="E1"/>
-    </sortState>
+  <autoFilter ref="B1:J246">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Calera De Víctor Rosales"/>
+      </filters>
+    </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>